<commit_message>
tambahan detail info penyelesaian proses
</commit_message>
<xml_diff>
--- a/Data/Output/fcfsOutput.xlsx
+++ b/Data/Output/fcfsOutput.xlsx
@@ -8,13 +8,14 @@
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="Sheet2" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="124519" fullCalcOnLoad="1"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="707" uniqueCount="376">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="712" uniqueCount="381">
   <si>
     <t>process</t>
   </si>
@@ -1142,6 +1143,21 @@
   </si>
   <si>
     <t>891</t>
+  </si>
+  <si>
+    <t>Total Process</t>
+  </si>
+  <si>
+    <t>AWT (Average Waiting Time)</t>
+  </si>
+  <si>
+    <t>Total Waiting Time</t>
+  </si>
+  <si>
+    <t>ATAT (Average Turn Around Time)</t>
+  </si>
+  <si>
+    <t>Total Turn Around Time</t>
   </si>
 </sst>
 </file>
@@ -3805,4 +3821,57 @@
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <dimension ref="A1:B5"/>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetData>
+    <row r="1" spans="1:2">
+      <c r="A1" t="s">
+        <v>376</v>
+      </c>
+      <c r="B1">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2">
+      <c r="A2" t="s">
+        <v>377</v>
+      </c>
+      <c r="B2">
+        <v>585.01</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2">
+      <c r="A3" t="s">
+        <v>378</v>
+      </c>
+      <c r="B3">
+        <v>58501</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2">
+      <c r="A4" t="s">
+        <v>379</v>
+      </c>
+      <c r="B4">
+        <v>597.59</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2">
+      <c r="A5" t="s">
+        <v>380</v>
+      </c>
+      <c r="B5">
+        <v>59759</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>